<commit_message>
Push pour le review 1
</commit_message>
<xml_diff>
--- a/V1/Gestion/Vérification_safety.xlsx
+++ b/V1/Gestion/Vérification_safety.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\rover_puissance\V1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\rover_puissance\V1\Gestion\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F2444AA-6D7D-4F17-A6EE-5F919B18D156}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7313EB-35E8-4B62-99F1-58E1461D7C9E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6465" yWindow="5355" windowWidth="15375" windowHeight="7875" xr2:uid="{F567074B-C168-4337-82A0-5B2E0A2AF515}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F567074B-C168-4337-82A0-5B2E0A2AF515}"/>
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>

</xml_diff>